<commit_message>
tests: migrated import page feature tests to pest
</commit_message>
<xml_diff>
--- a/tests/assets/PropertyImport.xlsx
+++ b/tests/assets/PropertyImport.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\swalbrun\repositories\solawi\tests\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA29E6D-90FF-4D4C-99E8-613955C23E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EFA29E6D-90FF-4D4C-99E8-613955C23E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47079AD2-7C28-4BCC-983E-6D101908DBAB}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C207C20-38C8-4794-BA5E-D2074C2481A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,19 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Property</t>
+    <t>PostName</t>
+  </si>
+  <si>
+    <t>BlogName</t>
   </si>
   <si>
     <t>PropsGehenRaus</t>
+  </si>
+  <si>
+    <t>KenBlock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,7 +115,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -407,34 +414,39 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="F3" s="2"/>

</xml_diff>